<commit_message>
add timesheet period Sep-Oct
</commit_message>
<xml_diff>
--- a/10_Period_20_Sep_2024_sd_19_Oct_2024/Timesheet Accord_Bayu Bagus Bagaswara_September-October.xlsx
+++ b/10_Period_20_Sep_2024_sd_19_Oct_2024/Timesheet Accord_Bayu Bagus Bagaswara_September-October.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bankdanamonindonesia-my.sharepoint.com/personal/v00028684_danamon_co_id/Documents/TIMESHEET BAYU/20240820_20240919/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bayub\Projects Bayu\TIMESHEET DANAMON BAYU\10_Period_20_Sep_2024_sd_19_Oct_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{843867E8-85EA-47E0-91B0-001AF53FAC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{056A5113-E682-4450-A0B2-8645B5536CB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{846D18A9-189A-468B-920E-4738CB6CEDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$AH$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Template!$A$1:$AG$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -28,7 +39,7 @@
     <author>securxcess</author>
   </authors>
   <commentList>
-    <comment ref="AI10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="AH10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -51,7 +62,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="AI10" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -79,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>TIME SHEET</t>
   </si>
@@ -164,16 +175,19 @@
     <t>Bayu Bagus Bagaswara</t>
   </si>
   <si>
-    <t>20 Agustus - 19 September</t>
-  </si>
-  <si>
-    <t>Discuss Release 9B - LKPBU &amp; LBABK</t>
-  </si>
-  <si>
-    <t>Development Release 9B - LKPBU &amp; LBABK</t>
-  </si>
-  <si>
-    <t>Monitoring Billing Statement</t>
+    <t>20 September - 19 October</t>
+  </si>
+  <si>
+    <t>Support SIT Release 9B - LKPBU &amp; LBABK</t>
+  </si>
+  <si>
+    <t>Support UAT Release 9B - LKPBU &amp; LBABK</t>
+  </si>
+  <si>
+    <t>Unit Testing Release 9B - LKPBU &amp; LBABK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Development Release 9B - LKPBU &amp; LBABK : - </t>
   </si>
 </sst>
 </file>
@@ -501,7 +515,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -642,9 +656,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -685,6 +696,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1073,27 +1096,27 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:EQ19"/>
+  <dimension ref="A1:EP20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="15.1796875" style="5" customWidth="1"/>
     <col min="2" max="2" width="42.54296875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="33" width="7.1796875" style="6" customWidth="1"/>
-    <col min="34" max="34" width="12" style="6" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="13.453125" style="6" customWidth="1"/>
-    <col min="36" max="36" width="14" style="6" customWidth="1"/>
-    <col min="37" max="37" width="11.81640625" style="6" customWidth="1"/>
-    <col min="38" max="38" width="14" style="6" customWidth="1"/>
-    <col min="39" max="39" width="12.54296875" style="6" customWidth="1"/>
-    <col min="40" max="16384" width="9.1796875" style="6"/>
+    <col min="3" max="32" width="7.1796875" style="6" customWidth="1"/>
+    <col min="33" max="33" width="12" style="6" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.453125" style="6" customWidth="1"/>
+    <col min="35" max="35" width="14" style="6" customWidth="1"/>
+    <col min="36" max="36" width="11.81640625" style="6" customWidth="1"/>
+    <col min="37" max="37" width="14" style="6" customWidth="1"/>
+    <col min="38" max="38" width="12.54296875" style="6" customWidth="1"/>
+    <col min="39" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:147" ht="29.25" customHeight="1">
+    <row r="1" spans="1:146" ht="29.25" customHeight="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1129,23 +1152,22 @@
       <c r="AE1" s="7"/>
       <c r="AF1" s="7"/>
       <c r="AG1" s="7"/>
-      <c r="AH1" s="7"/>
+      <c r="AH1" s="18"/>
       <c r="AI1" s="18"/>
       <c r="AJ1" s="18"/>
       <c r="AK1" s="18"/>
       <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
     </row>
-    <row r="2" spans="1:147" ht="25.5" customHeight="1">
-      <c r="AK2" s="19"/>
+    <row r="2" spans="1:146" ht="25.5" customHeight="1">
+      <c r="AJ2" s="19"/>
     </row>
-    <row r="3" spans="1:147" ht="25.5" customHeight="1">
-      <c r="AK3" s="19"/>
+    <row r="3" spans="1:146" ht="25.5" customHeight="1">
+      <c r="AJ3" s="19"/>
     </row>
-    <row r="4" spans="1:147" ht="25.5" customHeight="1">
-      <c r="AK4" s="19"/>
+    <row r="4" spans="1:146" ht="25.5" customHeight="1">
+      <c r="AJ4" s="19"/>
     </row>
-    <row r="5" spans="1:147" s="1" customFormat="1" ht="13.5" customHeight="1">
+    <row r="5" spans="1:146" s="1" customFormat="1" ht="13.5" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
@@ -1172,10 +1194,10 @@
       </c>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="66" t="s">
+      <c r="S5" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="T5" s="67"/>
+      <c r="T5" s="66"/>
       <c r="U5" s="10"/>
       <c r="V5" s="10" t="s">
         <v>24</v>
@@ -1190,62 +1212,60 @@
       <c r="AD5" s="10"/>
       <c r="AE5" s="10"/>
       <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="17"/>
       <c r="AI5" s="17"/>
-      <c r="AJ5" s="17"/>
     </row>
-    <row r="6" spans="1:147" s="2" customFormat="1" ht="75" customHeight="1">
+    <row r="6" spans="1:146" s="2" customFormat="1" ht="75" customHeight="1">
       <c r="A6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="B6" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="64"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="64"/>
-      <c r="N6" s="64"/>
-      <c r="O6" s="68" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="63"/>
+      <c r="N6" s="63"/>
+      <c r="O6" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="70"/>
-      <c r="S6" s="71">
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+      <c r="R6" s="69"/>
+      <c r="S6" s="70">
         <v>2024</v>
       </c>
-      <c r="T6" s="72"/>
-      <c r="U6" s="71" t="s">
+      <c r="T6" s="71"/>
+      <c r="U6" s="70" t="s">
         <v>25</v>
       </c>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="72"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="64"/>
+      <c r="X6" s="64"/>
+      <c r="Y6" s="64"/>
+      <c r="Z6" s="71"/>
       <c r="AA6" s="23"/>
-      <c r="AB6" s="65"/>
-      <c r="AC6" s="65"/>
-      <c r="AD6" s="65"/>
-      <c r="AE6" s="65"/>
+      <c r="AB6" s="64"/>
+      <c r="AC6" s="64"/>
+      <c r="AD6" s="64"/>
+      <c r="AE6" s="64"/>
       <c r="AF6" s="56"/>
-      <c r="AG6" s="56"/>
+      <c r="AG6" s="55"/>
       <c r="AH6" s="55"/>
-      <c r="AI6" s="55"/>
-      <c r="AJ6" s="24"/>
+      <c r="AI6" s="24"/>
     </row>
-    <row r="7" spans="1:147" s="1" customFormat="1" ht="15" customHeight="1">
+    <row r="7" spans="1:146" s="1" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="13"/>
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
@@ -1279,11 +1299,10 @@
       <c r="AE7" s="14"/>
       <c r="AF7" s="14"/>
       <c r="AG7" s="14"/>
-      <c r="AH7" s="14"/>
+      <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
-      <c r="AJ7" s="5"/>
     </row>
-    <row r="8" spans="1:147" ht="29.25" customHeight="1">
+    <row r="8" spans="1:146" ht="29.25" customHeight="1">
       <c r="A8" s="27" t="s">
         <v>7</v>
       </c>
@@ -1291,109 +1310,106 @@
         <v>8</v>
       </c>
       <c r="C8" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="H8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="29" t="s">
+      <c r="I8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="J8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="K8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="L8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="M8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="N8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="O8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="P8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="Q8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="R8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="S8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="29" t="s">
+      <c r="T8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="U8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="R8" s="29" t="s">
+      <c r="V8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="S8" s="29" t="s">
+      <c r="W8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="T8" s="29" t="s">
+      <c r="X8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="U8" s="29" t="s">
+      <c r="Y8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="V8" s="29" t="s">
+      <c r="Z8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="W8" s="29" t="s">
+      <c r="AA8" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="X8" s="29" t="s">
+      <c r="AB8" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="Y8" s="29" t="s">
+      <c r="AC8" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="Z8" s="29" t="s">
+      <c r="AD8" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="29" t="s">
+      <c r="AE8" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="AB8" s="29" t="s">
+      <c r="AF8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="AC8" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="AD8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="AE8" s="29" t="s">
-        <v>10</v>
-      </c>
-      <c r="AF8" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="AG8" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH8" s="51" t="s">
+      <c r="AG8" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="AI8" s="30" t="s">
+      <c r="AH8" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="AJ8" s="31" t="s">
+      <c r="AI8" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:147" ht="21.75" customHeight="1">
+    <row r="9" spans="1:146" ht="21.75" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="33"/>
       <c r="C9" s="48">
@@ -1430,70 +1446,67 @@
         <v>30</v>
       </c>
       <c r="N9" s="48">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="O9" s="48">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P9" s="48">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Q9" s="48">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R9" s="48">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="S9" s="48">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="T9" s="48">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="U9" s="48">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V9" s="48">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W9" s="48">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="X9" s="48">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y9" s="48">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Z9" s="48">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA9" s="48">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AB9" s="48">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AC9" s="48">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AD9" s="48">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AE9" s="48">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AF9" s="48">
-        <v>18</v>
-      </c>
-      <c r="AG9" s="48">
         <v>19</v>
       </c>
-      <c r="AH9" s="46"/>
-      <c r="AI9" s="30"/>
-      <c r="AJ9" s="34"/>
+      <c r="AG9" s="46"/>
+      <c r="AH9" s="30"/>
+      <c r="AI9" s="34"/>
     </row>
-    <row r="10" spans="1:147" s="3" customFormat="1" ht="33" customHeight="1">
+    <row r="10" spans="1:146" s="3" customFormat="1" ht="33" customHeight="1">
       <c r="A10" s="35"/>
       <c r="B10" s="26" t="s">
         <v>22</v>
@@ -1501,86 +1514,84 @@
       <c r="C10" s="57">
         <v>1</v>
       </c>
-      <c r="D10" s="57">
-        <v>1</v>
-      </c>
-      <c r="E10" s="57">
-        <v>1</v>
-      </c>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
       <c r="F10" s="57">
         <v>1</v>
       </c>
-      <c r="G10" s="52"/>
-      <c r="H10" s="52"/>
+      <c r="G10" s="72">
+        <v>1</v>
+      </c>
+      <c r="H10" s="72">
+        <v>1</v>
+      </c>
       <c r="I10" s="57">
         <v>1</v>
       </c>
       <c r="J10" s="57">
         <v>1</v>
       </c>
-      <c r="K10" s="57">
-        <v>1</v>
-      </c>
-      <c r="L10" s="57">
-        <v>1</v>
-      </c>
+      <c r="K10" s="52"/>
+      <c r="L10" s="52"/>
       <c r="M10" s="57">
         <v>1</v>
       </c>
-      <c r="N10" s="52"/>
-      <c r="O10" s="52"/>
+      <c r="N10" s="72">
+        <v>1</v>
+      </c>
+      <c r="O10" s="72">
+        <v>1</v>
+      </c>
       <c r="P10" s="57">
         <v>1</v>
       </c>
       <c r="Q10" s="57">
         <v>1</v>
       </c>
-      <c r="R10" s="57">
-        <v>1</v>
-      </c>
-      <c r="S10" s="57">
-        <v>1</v>
-      </c>
+      <c r="R10" s="52"/>
+      <c r="S10" s="52"/>
       <c r="T10" s="57">
         <v>1</v>
       </c>
-      <c r="U10" s="52"/>
-      <c r="V10" s="52"/>
+      <c r="U10" s="72">
+        <v>1</v>
+      </c>
+      <c r="V10" s="72">
+        <v>1</v>
+      </c>
       <c r="W10" s="57">
         <v>1</v>
       </c>
       <c r="X10" s="57">
         <v>1</v>
       </c>
-      <c r="Y10" s="57">
-        <v>1</v>
-      </c>
-      <c r="Z10" s="57">
-        <v>1</v>
-      </c>
+      <c r="Y10" s="52"/>
+      <c r="Z10" s="52"/>
       <c r="AA10" s="57">
         <v>1</v>
       </c>
-      <c r="AB10" s="52"/>
-      <c r="AC10" s="52"/>
-      <c r="AD10" s="53"/>
+      <c r="AB10" s="72">
+        <v>1</v>
+      </c>
+      <c r="AC10" s="72">
+        <v>1</v>
+      </c>
+      <c r="AD10" s="73">
+        <v>1</v>
+      </c>
       <c r="AE10" s="49">
         <v>1</v>
       </c>
-      <c r="AF10" s="49">
-        <v>1</v>
-      </c>
-      <c r="AG10" s="49">
-        <v>1</v>
-      </c>
-      <c r="AH10" s="44">
-        <f>SUM(C10:AG10)</f>
-        <v>22</v>
-      </c>
-      <c r="AI10" s="59" t="s">
+      <c r="AF10" s="53"/>
+      <c r="AG10" s="44">
+        <f>SUM(C10:AF10)</f>
+        <v>21</v>
+      </c>
+      <c r="AH10" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="AJ10" s="61"/>
+      <c r="AI10" s="60"/>
+      <c r="AJ10" s="6"/>
       <c r="AK10" s="6"/>
       <c r="AL10" s="6"/>
       <c r="AM10" s="6"/>
@@ -1691,421 +1702,419 @@
       <c r="EN10" s="6"/>
       <c r="EO10" s="6"/>
       <c r="EP10" s="6"/>
-      <c r="EQ10" s="6"/>
     </row>
-    <row r="11" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="11" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A11" s="36"/>
       <c r="B11" s="47" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C11" s="49">
-        <v>2</v>
-      </c>
-      <c r="D11" s="49">
-        <v>2</v>
-      </c>
-      <c r="E11" s="58">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="D11" s="53"/>
+      <c r="E11" s="75"/>
       <c r="F11" s="49">
-        <v>2</v>
-      </c>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
+        <v>7</v>
+      </c>
+      <c r="G11" s="73">
+        <v>7</v>
+      </c>
+      <c r="H11" s="73">
+        <v>7</v>
+      </c>
       <c r="I11" s="49">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J11" s="49">
-        <v>2</v>
-      </c>
-      <c r="K11" s="49">
-        <v>2</v>
-      </c>
-      <c r="L11" s="49">
-        <v>2</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
       <c r="M11" s="49">
-        <v>2</v>
-      </c>
-      <c r="N11" s="53"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="49">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="49">
-        <v>2</v>
-      </c>
-      <c r="R11" s="49">
-        <v>2</v>
-      </c>
-      <c r="S11" s="49">
-        <v>2</v>
-      </c>
-      <c r="T11" s="49">
-        <v>2</v>
-      </c>
-      <c r="U11" s="53"/>
-      <c r="V11" s="53"/>
-      <c r="W11" s="49">
-        <v>2</v>
-      </c>
-      <c r="X11" s="49">
-        <v>2</v>
-      </c>
-      <c r="Y11" s="49">
-        <v>2</v>
-      </c>
-      <c r="Z11" s="49">
-        <v>2</v>
-      </c>
-      <c r="AA11" s="49">
-        <v>2</v>
-      </c>
-      <c r="AB11" s="53"/>
-      <c r="AC11" s="53"/>
-      <c r="AD11" s="53"/>
-      <c r="AE11" s="49">
-        <v>2</v>
-      </c>
-      <c r="AF11" s="49">
-        <v>2</v>
-      </c>
-      <c r="AG11" s="49">
-        <v>2</v>
-      </c>
-      <c r="AH11" s="44">
-        <f>SUM(C11:AG11)</f>
-        <v>44</v>
-      </c>
-      <c r="AI11" s="60"/>
-      <c r="AJ11" s="62"/>
+        <v>4</v>
+      </c>
+      <c r="N11" s="73">
+        <v>4</v>
+      </c>
+      <c r="O11" s="73"/>
+      <c r="P11" s="49"/>
+      <c r="Q11" s="49"/>
+      <c r="R11" s="53"/>
+      <c r="S11" s="53"/>
+      <c r="T11" s="49"/>
+      <c r="U11" s="73"/>
+      <c r="V11" s="73"/>
+      <c r="W11" s="49"/>
+      <c r="X11" s="49"/>
+      <c r="Y11" s="53"/>
+      <c r="Z11" s="53"/>
+      <c r="AA11" s="49"/>
+      <c r="AB11" s="73"/>
+      <c r="AC11" s="73"/>
+      <c r="AD11" s="73"/>
+      <c r="AE11" s="49"/>
+      <c r="AF11" s="53"/>
+      <c r="AG11" s="44">
+        <f>SUM(C11:AF11)</f>
+        <v>48</v>
+      </c>
+      <c r="AH11" s="59"/>
+      <c r="AI11" s="61"/>
     </row>
-    <row r="12" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="12" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A12" s="36"/>
       <c r="B12" s="47" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="49">
-        <v>5</v>
-      </c>
-      <c r="D12" s="49">
-        <v>5</v>
-      </c>
-      <c r="E12" s="58">
-        <v>5</v>
-      </c>
-      <c r="F12" s="49">
-        <v>5</v>
-      </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
+        <v>30</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="53"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="73"/>
+      <c r="H12" s="73"/>
       <c r="I12" s="49">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J12" s="49">
-        <v>5</v>
-      </c>
-      <c r="K12" s="49">
-        <v>5</v>
-      </c>
-      <c r="L12" s="49">
-        <v>5</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K12" s="53"/>
+      <c r="L12" s="53"/>
       <c r="M12" s="49">
-        <v>5</v>
-      </c>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="49">
+        <v>3</v>
+      </c>
+      <c r="N12" s="73">
+        <v>3</v>
+      </c>
+      <c r="O12" s="73">
         <v>4</v>
       </c>
-      <c r="Q12" s="49">
-        <v>5</v>
-      </c>
-      <c r="R12" s="49">
-        <v>5</v>
-      </c>
-      <c r="S12" s="49">
-        <v>5</v>
-      </c>
-      <c r="T12" s="49">
-        <v>5</v>
-      </c>
-      <c r="U12" s="53"/>
-      <c r="V12" s="53"/>
-      <c r="W12" s="49">
-        <v>4</v>
-      </c>
-      <c r="X12" s="49">
-        <v>5</v>
-      </c>
-      <c r="Y12" s="49">
-        <v>5</v>
-      </c>
-      <c r="Z12" s="49">
-        <v>5</v>
-      </c>
-      <c r="AA12" s="49">
-        <v>5</v>
-      </c>
-      <c r="AB12" s="53"/>
-      <c r="AC12" s="53"/>
-      <c r="AD12" s="53"/>
-      <c r="AE12" s="49">
-        <v>4</v>
-      </c>
-      <c r="AF12" s="49">
-        <v>5</v>
-      </c>
-      <c r="AG12" s="49">
-        <v>5</v>
-      </c>
-      <c r="AH12" s="44">
-        <f>SUM(C12:AG12)</f>
-        <v>107</v>
-      </c>
-      <c r="AI12" s="60"/>
-      <c r="AJ12" s="62"/>
+      <c r="P12" s="49"/>
+      <c r="Q12" s="49"/>
+      <c r="R12" s="53"/>
+      <c r="S12" s="53"/>
+      <c r="T12" s="49"/>
+      <c r="U12" s="73"/>
+      <c r="V12" s="73"/>
+      <c r="W12" s="49"/>
+      <c r="X12" s="49"/>
+      <c r="Y12" s="53"/>
+      <c r="Z12" s="53"/>
+      <c r="AA12" s="49"/>
+      <c r="AB12" s="73"/>
+      <c r="AC12" s="73"/>
+      <c r="AD12" s="73"/>
+      <c r="AE12" s="49"/>
+      <c r="AF12" s="53"/>
+      <c r="AG12" s="44">
+        <f>SUM(C12:AF12)</f>
+        <v>12</v>
+      </c>
+      <c r="AH12" s="59"/>
+      <c r="AI12" s="61"/>
     </row>
-    <row r="13" spans="1:147" s="4" customFormat="1" ht="33" customHeight="1">
+    <row r="13" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
       <c r="A13" s="36"/>
       <c r="B13" s="47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="58"/>
+      <c r="D13" s="53"/>
+      <c r="E13" s="75"/>
       <c r="F13" s="49"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="53"/>
+      <c r="G13" s="73"/>
+      <c r="H13" s="73"/>
       <c r="I13" s="49"/>
       <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="49"/>
+      <c r="K13" s="53"/>
+      <c r="L13" s="53"/>
       <c r="M13" s="49"/>
-      <c r="N13" s="53"/>
-      <c r="O13" s="53"/>
+      <c r="N13" s="73"/>
+      <c r="O13" s="73">
+        <v>3</v>
+      </c>
       <c r="P13" s="49">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="49"/>
-      <c r="R13" s="49"/>
-      <c r="S13" s="49"/>
-      <c r="T13" s="49"/>
-      <c r="U13" s="53"/>
-      <c r="V13" s="53"/>
+        <v>4</v>
+      </c>
+      <c r="Q13" s="49">
+        <v>5</v>
+      </c>
+      <c r="R13" s="53"/>
+      <c r="S13" s="53"/>
+      <c r="T13" s="49">
+        <v>7</v>
+      </c>
+      <c r="U13" s="73">
+        <v>7</v>
+      </c>
+      <c r="V13" s="73">
+        <v>7</v>
+      </c>
       <c r="W13" s="49">
-        <v>1</v>
-      </c>
-      <c r="X13" s="49"/>
-      <c r="Y13" s="49"/>
-      <c r="Z13" s="49"/>
-      <c r="AA13" s="49"/>
-      <c r="AB13" s="53"/>
-      <c r="AC13" s="53"/>
-      <c r="AD13" s="53"/>
-      <c r="AE13" s="49">
-        <v>1</v>
-      </c>
-      <c r="AF13" s="49"/>
-      <c r="AG13" s="49"/>
-      <c r="AH13" s="44">
-        <f>SUM(C13:AG13)</f>
+        <v>7</v>
+      </c>
+      <c r="X13" s="49">
+        <v>4</v>
+      </c>
+      <c r="Y13" s="53"/>
+      <c r="Z13" s="53"/>
+      <c r="AA13" s="49">
+        <v>2</v>
+      </c>
+      <c r="AB13" s="73">
+        <v>2</v>
+      </c>
+      <c r="AC13" s="73"/>
+      <c r="AD13" s="73"/>
+      <c r="AE13" s="49"/>
+      <c r="AF13" s="53"/>
+      <c r="AG13" s="44">
+        <f>SUM(C13:AF13)</f>
+        <v>48</v>
+      </c>
+      <c r="AH13" s="59"/>
+      <c r="AI13" s="61"/>
+    </row>
+    <row r="14" spans="1:146" s="4" customFormat="1" ht="33" customHeight="1">
+      <c r="A14" s="36"/>
+      <c r="B14" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="49"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="73"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="49"/>
+      <c r="N14" s="73"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="49"/>
+      <c r="Q14" s="49"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="49"/>
+      <c r="U14" s="73"/>
+      <c r="V14" s="73"/>
+      <c r="W14" s="49"/>
+      <c r="X14" s="49">
         <v>3</v>
       </c>
-      <c r="AI13" s="60"/>
-      <c r="AJ13" s="62"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="49">
+        <v>5</v>
+      </c>
+      <c r="AB14" s="73">
+        <v>5</v>
+      </c>
+      <c r="AC14" s="73">
+        <v>7</v>
+      </c>
+      <c r="AD14" s="73">
+        <v>7</v>
+      </c>
+      <c r="AE14" s="49">
+        <v>7</v>
+      </c>
+      <c r="AF14" s="53"/>
+      <c r="AG14" s="44">
+        <f>SUM(C14:AF14)</f>
+        <v>34</v>
+      </c>
+      <c r="AH14" s="59"/>
+      <c r="AI14" s="61"/>
     </row>
-    <row r="14" spans="1:147" s="4" customFormat="1" ht="36" customHeight="1">
-      <c r="A14" s="37" t="s">
+    <row r="15" spans="1:146" s="4" customFormat="1" ht="36" customHeight="1">
+      <c r="A15" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="50">
-        <f t="shared" ref="C14:AG14" si="0">SUM(C10:C13)</f>
+      <c r="B15" s="38"/>
+      <c r="C15" s="50">
+        <f>SUM(C10:C14)</f>
         <v>8</v>
       </c>
-      <c r="D14" s="50">
+      <c r="D15" s="50">
+        <f t="shared" ref="D15:G15" si="0">SUM(D10:D14)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F15" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E14" s="50">
+      <c r="G15" s="50">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F14" s="50">
-        <f t="shared" si="0"/>
+      <c r="H15" s="74">
+        <f>SUM(H10:H14)</f>
         <v>8</v>
       </c>
-      <c r="G14" s="54">
-        <f t="shared" si="0"/>
+      <c r="I15" s="50">
+        <f>SUM(I10:I14)</f>
+        <v>8</v>
+      </c>
+      <c r="J15" s="50">
+        <f>SUM(J10:J14)</f>
+        <v>8</v>
+      </c>
+      <c r="K15" s="54">
+        <f>SUM(K10:K14)</f>
         <v>0</v>
       </c>
-      <c r="H14" s="54">
-        <f t="shared" si="0"/>
+      <c r="L15" s="54">
+        <f>SUM(L10:L14)</f>
         <v>0</v>
       </c>
-      <c r="I14" s="50">
-        <f t="shared" si="0"/>
+      <c r="M15" s="50">
+        <f>SUM(M10:M14)</f>
         <v>8</v>
       </c>
-      <c r="J14" s="50">
-        <f t="shared" si="0"/>
+      <c r="N15" s="74">
+        <f>SUM(N10:N14)</f>
         <v>8</v>
       </c>
-      <c r="K14" s="50">
-        <f t="shared" si="0"/>
+      <c r="O15" s="74">
+        <f>SUM(O10:O14)</f>
         <v>8</v>
       </c>
-      <c r="L14" s="50">
-        <f t="shared" si="0"/>
+      <c r="P15" s="50">
+        <f>SUM(P10:P14)</f>
+        <v>5</v>
+      </c>
+      <c r="Q15" s="50">
+        <f>SUM(Q10:Q14)</f>
+        <v>6</v>
+      </c>
+      <c r="R15" s="54">
+        <f>SUM(R10:R14)</f>
+        <v>0</v>
+      </c>
+      <c r="S15" s="54">
+        <f>SUM(S10:S14)</f>
+        <v>0</v>
+      </c>
+      <c r="T15" s="50">
+        <f>SUM(T10:T14)</f>
         <v>8</v>
       </c>
-      <c r="M14" s="50">
-        <f t="shared" si="0"/>
+      <c r="U15" s="74">
+        <f>SUM(U10:U14)</f>
         <v>8</v>
       </c>
-      <c r="N14" s="54">
-        <f t="shared" si="0"/>
+      <c r="V15" s="74">
+        <f>SUM(V10:V14)</f>
+        <v>8</v>
+      </c>
+      <c r="W15" s="50">
+        <f>SUM(W10:W14)</f>
+        <v>8</v>
+      </c>
+      <c r="X15" s="50">
+        <f>SUM(X10:X14)</f>
+        <v>8</v>
+      </c>
+      <c r="Y15" s="54">
+        <f>SUM(Y10:Y14)</f>
         <v>0</v>
       </c>
-      <c r="O14" s="54">
-        <f t="shared" si="0"/>
+      <c r="Z15" s="54">
+        <f>SUM(Z10:Z14)</f>
         <v>0</v>
       </c>
-      <c r="P14" s="50">
-        <f t="shared" si="0"/>
+      <c r="AA15" s="50">
+        <f>SUM(AA10:AA14)</f>
         <v>8</v>
       </c>
-      <c r="Q14" s="50">
-        <f t="shared" si="0"/>
+      <c r="AB15" s="74">
+        <f>SUM(AB10:AB14)</f>
         <v>8</v>
       </c>
-      <c r="R14" s="50">
-        <f t="shared" si="0"/>
+      <c r="AC15" s="74">
+        <f>SUM(AC10:AC14)</f>
         <v>8</v>
       </c>
-      <c r="S14" s="50">
-        <f t="shared" si="0"/>
+      <c r="AD15" s="74">
+        <f>SUM(AD10:AD14)</f>
         <v>8</v>
       </c>
-      <c r="T14" s="50">
-        <f t="shared" si="0"/>
+      <c r="AE15" s="50">
+        <f>SUM(AE10:AE14)</f>
         <v>8</v>
       </c>
-      <c r="U14" s="54">
-        <f t="shared" si="0"/>
+      <c r="AF15" s="54">
+        <f>SUM(AF10:AF14)</f>
         <v>0</v>
       </c>
-      <c r="V14" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="W14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="X14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Y14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="Z14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AA14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AB14" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AC14" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AD14" s="54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="AE14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AF14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AG14" s="50">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AH14" s="45">
-        <f>SUM(C14:AG14)</f>
-        <v>176</v>
-      </c>
-      <c r="AI14" s="39"/>
-      <c r="AJ14" s="40"/>
+      <c r="AG15" s="45">
+        <f>SUM(C15:AF15)</f>
+        <v>163</v>
+      </c>
+      <c r="AH15" s="39"/>
+      <c r="AI15" s="40"/>
     </row>
-    <row r="15" spans="1:147" ht="23.25" customHeight="1">
-      <c r="A15" s="41" t="s">
+    <row r="16" spans="1:146" ht="23.25" customHeight="1">
+      <c r="A16" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
-      <c r="N15" s="42"/>
-      <c r="O15" s="42"/>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
-      <c r="U15" s="43"/>
-      <c r="V15" s="42"/>
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="42"/>
+      <c r="L16" s="42"/>
+      <c r="M16" s="42"/>
+      <c r="N16" s="42"/>
+      <c r="O16" s="42"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="42"/>
+      <c r="R16" s="42"/>
+      <c r="S16" s="42"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="43"/>
+      <c r="V16" s="42"/>
     </row>
-    <row r="16" spans="1:147">
-      <c r="A16" s="15"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
+    <row r="17" spans="1:26" ht="14.5">
+      <c r="A17" s="15"/>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16"/>
+      <c r="I17" s="16"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="16"/>
+      <c r="L17" s="16"/>
+      <c r="M17" s="16"/>
     </row>
-    <row r="17" spans="26:26" ht="16">
-      <c r="Z17" s="21"/>
+    <row r="18" spans="1:26">
+      <c r="Z18" s="21"/>
     </row>
-    <row r="18" spans="26:26">
-      <c r="Z18" s="22"/>
+    <row r="19" spans="1:26">
+      <c r="Z19" s="22"/>
     </row>
-    <row r="19" spans="26:26" ht="12.75" customHeight="1">
-      <c r="Z19" s="22"/>
+    <row r="20" spans="1:26" ht="12.75" customHeight="1">
+      <c r="Z20" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="AI10:AI13"/>
-    <mergeCell ref="AJ10:AJ13"/>
+    <mergeCell ref="AH10:AH14"/>
+    <mergeCell ref="AI10:AI14"/>
     <mergeCell ref="C6:N6"/>
     <mergeCell ref="AB6:AE6"/>
     <mergeCell ref="S5:T5"/>

</xml_diff>